<commit_message>
handled the nan value and extracted data into files
</commit_message>
<xml_diff>
--- a/data_and_files/MatlabCodes/zhiye_vars.xlsx
+++ b/data_and_files/MatlabCodes/zhiye_vars.xlsx
@@ -26,6 +26,118 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
+    <t>一次加料累计精度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次加水流量（l/h）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次后端蒸汽温度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次后端阀前蒸汽压力（bar）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次液料流量（kg/h）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次筒转速（l/min）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一次除尘房排潮风机频率（HZ）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次前端蒸汽体积流量（m3/h）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次前端蒸汽温度（℃）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次前端蒸汽薄膜阀开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次加料泵开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次后端蒸汽温度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次后端蒸汽薄膜阀开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二次液料累计量（kg）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散出口水分（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散前端加水流量（l/h）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散后端加水流量（l/h）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散后端加水累计量（l）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散后端加水薄膜阀开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散排潮负压开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散排潮负压（mbar）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散新风蒸汽阀门开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散新风风门开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散热风温度（℃）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散热风蒸汽阀门开度（%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散蒸汽质量流量（kg/h）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松散除尘房排潮风机频率（HZ）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>片烟流量（kg/h）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>一次1#罐料液温度（℃）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,14 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一次加料累计精度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一次加水流量（l/h）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一次加水累计量（l）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -90,10 +194,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一次后端蒸汽温度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一次后端蒸汽薄膜阀开度（%）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -102,14 +202,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一次后端阀前蒸汽压力（bar）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一次液料流量（kg/h）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一次液料累计量（kg）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -126,14 +218,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一次筒转速（l/min）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一次除尘房排潮风机频率（HZ）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>二次入口水分（%）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -146,18 +230,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>二次前端蒸汽体积流量（m3/h）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二次前端蒸汽温度（℃）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二次前端蒸汽薄膜阀开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>二次前端蒸汽质量流量（kg/h）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -166,10 +238,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>二次加料泵开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>二次加料瞬时比例（%）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,14 +262,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>二次后端蒸汽温度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二次后端蒸汽薄膜阀开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>二次后端蒸汽质量流量（%）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -214,10 +274,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>二次液料累计量（kg）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>二次烟叶流量（kg/h）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -238,18 +294,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>松散出口水分（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>松散出口温度（℃）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>松散前端加水流量（l/h）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>松散前端加水累计量（l）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -258,26 +306,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>松散后端加水流量（l/h）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>松散后端加水累计量（l）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>松散后端加水薄膜阀开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>松散排潮负压开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>松散排潮负压（mbar）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>松散新增热风温度（℃）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -286,26 +314,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>松散新风蒸汽阀门开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>松散新风风门开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>松散滚筒转速（l/min）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>松散热风温度（℃）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>松散热风蒸汽阀门开度（%）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>松散热风风门开度（%）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -318,23 +330,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>松散蒸汽质量流量（kg/h）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>松散阀前蒸汽压力（bar）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>松散阀前蒸汽温度（℃）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>松散除尘房排潮风机频率（HZ）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>片烟流量（kg/h）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -677,392 +677,392 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>